<commit_message>
Improve: Enhance audio file metadata template with clear headers, example data, styling, and instructions sheet for improved usability.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 2e616067-30d1-4cf8-b9ac-91a12608fb44
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/99e565d9-defe-4b43-9370-4d17ce50e7be/cd38fb9d-0e29-4757-8456-b0ed967aaaa9.jpg
</commit_message>
<xml_diff>
--- a/public/templates/audio_files_metadata_template.xlsx
+++ b/public/templates/audio_files_metadata_template.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Audio Files Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -401,6 +402,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -453,10 +465,10 @@
       <c r="G2" t="str">
         <v>CALL789</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="str">
         <v>4</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="str">
         <v>180</v>
       </c>
     </row>
@@ -482,10 +494,10 @@
       <c r="G3" t="str">
         <v>CALL456</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="str">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="str">
         <v>240</v>
       </c>
     </row>
@@ -494,4 +506,119 @@
     <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Audio File Metadata - Instructions</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>This template is used to provide metadata for audio files in batch uploads.</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Field Instructions:</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>filename</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Must match the exact filename of the uploaded audio file (including extension)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>language</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Use one of: english, spanish, french, hindi, other</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>version</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Version number or identifier of the call script/process used</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>call_date</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Date of the call in YYYY-MM-DD format</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>call_type</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Type of call, e.g., inbound, outbound, service, sales, etc.</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>agent_id</v>
+      </c>
+      <c r="B11" t="str">
+        <v>ID of the agent who handled the call</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>call_id</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Unique identifier of the call (if available)</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>customer_satisfaction</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Customer satisfaction score, typically 1-5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>handle_time</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Call duration in seconds</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B14"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>